<commit_message>
changes to feedback form
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -471,13 +471,10 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>42</v>
-      </c>
-      <c r="D2">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -485,13 +482,10 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>58</v>
-      </c>
-      <c r="D3">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -499,13 +493,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>91</v>
-      </c>
-      <c r="D4">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -513,13 +504,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>102</v>
-      </c>
-      <c r="D5">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -527,13 +515,10 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>89</v>
-      </c>
-      <c r="D6">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -541,13 +526,10 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>45</v>
-      </c>
-      <c r="D7">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -555,13 +537,10 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>62</v>
-      </c>
-      <c r="D8">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -569,13 +548,10 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>47</v>
-      </c>
-      <c r="D9">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -584,15 +560,14 @@
       </c>
       <c r="B13">
         <f>SUBTOTAL(109,B2:B12)</f>
-        <v>112</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <f>SUBTOTAL(109,C2:C12)</f>
         <v>536</v>
       </c>
       <c r="D13">
-        <f>SUBTOTAL(109,D2:D12)</f>
-        <v>322</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>